<commit_message>
kmk - InGame Ani1
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\카카오톡 받은 파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE94049-ADF5-4D6F-BD60-3F47A474F51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6143B8FB-8E1E-418C-850B-385FBF00EDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="18816" tabRatio="855" activeTab="3" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
+    <workbookView xWindow="11856" yWindow="2316" windowWidth="29592" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="8" r:id="rId1"/>
@@ -1598,10 +1598,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5559,30 +5559,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="53"/>
+      <c r="F4" s="54"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="54"/>
     </row>
     <row r="5" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
@@ -5691,10 +5691,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="18"/>
       <c r="E10" s="14" t="s">
         <v>16</v>
@@ -5748,10 +5748,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="53"/>
+      <c r="F13" s="54"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5800,10 +5800,10 @@
         <v>35</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="53"/>
+      <c r="F17" s="54"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -5841,10 +5841,10 @@
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="54"/>
       <c r="D20" s="18"/>
       <c r="E20" s="14" t="s">
         <v>40</v>
@@ -5968,15 +5968,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5988,8 +5988,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6276,7 +6276,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
kmk - gamePlay Ani
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6143B8FB-8E1E-418C-850B-385FBF00EDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04670DAF-C044-4975-99AD-6909ABFE32EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11856" yWindow="2316" windowWidth="29592" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="217">
   <si>
     <t>stage1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1598,10 +1598,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5559,30 +5559,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="54"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="54"/>
+      <c r="F4" s="53"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="54" t="s">
+      <c r="H4" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="54"/>
+      <c r="I4" s="53"/>
     </row>
     <row r="5" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
@@ -5691,10 +5691,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="18"/>
       <c r="E10" s="14" t="s">
         <v>16</v>
@@ -5748,10 +5748,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="54"/>
+      <c r="F13" s="53"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5800,10 +5800,10 @@
         <v>35</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="54" t="s">
+      <c r="E17" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="54"/>
+      <c r="F17" s="53"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -5841,10 +5841,10 @@
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="54"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="18"/>
       <c r="E20" s="14" t="s">
         <v>40</v>
@@ -5968,15 +5968,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5989,7 +5989,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6061,13 +6061,15 @@
       </c>
       <c r="C2" s="11">
         <f>COUNTA(표14[[#This Row],[enemy_unit1]:[enemy_unit3]])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="11" t="str">
         <f>monster_ref!$B$4</f>
         <v>스켈레톤</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>182</v>
+      </c>
       <c r="F2" s="51"/>
       <c r="G2" s="48">
         <v>0</v>

</xml_diff>

<commit_message>
kmk - gamePlay UI 2
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76466D5B-0ABD-4BA7-8F46-C7F36FB88D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCFA2B1-F133-4787-90BC-6ADEE608EB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11856" yWindow="2316" windowWidth="29592" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="217">
   <si>
     <t>stage1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1598,13 +1598,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5559,30 +5559,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="53"/>
+      <c r="F4" s="54"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="54"/>
     </row>
     <row r="5" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
@@ -5691,10 +5691,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="18"/>
       <c r="E10" s="14" t="s">
         <v>16</v>
@@ -5748,10 +5748,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="53"/>
+      <c r="F13" s="54"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5783,10 +5783,10 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -5800,10 +5800,10 @@
         <v>35</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="53"/>
+      <c r="F17" s="54"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -5841,10 +5841,10 @@
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="54"/>
       <c r="D20" s="18"/>
       <c r="E20" s="14" t="s">
         <v>40</v>
@@ -5968,6 +5968,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
@@ -5975,8 +5977,6 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5989,7 +5989,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6061,13 +6061,15 @@
       </c>
       <c r="C2" s="11">
         <f>COUNTA(표14[[#This Row],[enemy_unit1]:[enemy_unit3]])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="11" t="str">
         <f>monster_ref!$B$4</f>
         <v>스켈레톤</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>182</v>
+      </c>
       <c r="F2" s="51"/>
       <c r="G2" s="48">
         <v>0</v>

</xml_diff>

<commit_message>
kmk effect_add and bug fix
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\만두~\게임 프로젝트\4) 2023.10 ~ 2023.12 인턴 프로젝트\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3534B414-69AE-4284-BC02-544EC1D013F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DABABE8-48B5-4683-97E9-ED41F730A1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11856" yWindow="2316" windowWidth="29592" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
+    <workbookView xWindow="30612" yWindow="1800" windowWidth="23256" windowHeight="12576" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="217">
   <si>
     <t>stage1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1601,10 +1601,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1616,10 +1616,6 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="68">
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2306,6 +2302,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4629,7 +4629,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="몬스터"/>
@@ -4821,24 +4821,24 @@
     </tableColumn>
     <tableColumn id="4" xr3:uid="{56F412A6-1D1C-4DD8-8F9F-A9D6D5CB1F01}" name="enemy_unit1" dataDxfId="52"/>
     <tableColumn id="5" xr3:uid="{E89A1493-B142-49A1-9C5F-0140455DF9CD}" name="enemy_unit2" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{822F2BAA-16F4-4BC6-9BCB-01758A14B4CF}" name="enemy_unit3" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{822F2BAA-16F4-4BC6-9BCB-01758A14B4CF}" name="enemy_unit3" dataDxfId="50">
       <calculatedColumnFormula>표3[[#This Row],[name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{08FE4F30-2D1A-48D4-B845-F2EF9F32375F}" name="reward_hp" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{09318C06-AB06-4E71-AAD3-53C176D856D4}" name="reward_point" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{DC5BC79E-8C2D-4FB9-BF6E-051A19757C96}" name="reward_coin" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{9ACB5939-E1BD-48F3-8490-09A8DF246598}" name="open_item" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{6988D6FA-4BE7-4E74-B798-7FF44AD473F7}" name="image" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{08CE1504-5F64-4F38-8E02-BA3C4A127ACB}" name="sound" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{16AC2542-0BB8-4573-B0D6-E7FC48FC2FF0}" name="stage_fullname" dataDxfId="44"/>
-    <tableColumn id="14" xr3:uid="{CC2A6C46-331D-4AA2-B4BA-67EC194D8A2F}" name="stage_info" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{08FE4F30-2D1A-48D4-B845-F2EF9F32375F}" name="reward_hp" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{09318C06-AB06-4E71-AAD3-53C176D856D4}" name="reward_point" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{DC5BC79E-8C2D-4FB9-BF6E-051A19757C96}" name="reward_coin" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{9ACB5939-E1BD-48F3-8490-09A8DF246598}" name="open_item" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{6988D6FA-4BE7-4E74-B798-7FF44AD473F7}" name="image" dataDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{08CE1504-5F64-4F38-8E02-BA3C4A127ACB}" name="sound" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{16AC2542-0BB8-4573-B0D6-E7FC48FC2FF0}" name="stage_fullname" dataDxfId="43"/>
+    <tableColumn id="14" xr3:uid="{CC2A6C46-331D-4AA2-B4BA-67EC194D8A2F}" name="stage_info" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}" name="표3" displayName="표3" ref="A1:J7" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}" name="표3" displayName="표3" ref="A1:J7" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:J7" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4852,47 +4852,47 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{38E8F74F-24B3-44C3-8D51-9ED44863F676}" name="id" totalsRowLabel="요약" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{E272DE11-2CFA-438A-8C30-4093EEBAAD4D}" name="name" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{2CF08806-9622-4698-9F29-63005B4ACF6B}" name="name_en" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{494873D0-DE71-4A7C-A5C1-1CD13F2D633F}" name="type" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{354215F0-D267-44D0-B417-9824FD6469DC}" name="hp" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{B4511A73-E29D-4385-AE5F-8C007E1D956D}" name="atk" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{C37631EF-1FE2-449B-8ADB-3FC65C48BB02}" name="def" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{47878641-5549-4C24-8792-3F626D6AFFF8}" name="image" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{2DFA05EF-9697-418B-B5C7-E4A0E66783E9}" name="sound" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{105408C5-D9C0-44F0-A870-D9BE4782B17F}" name="enemy_info" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{38E8F74F-24B3-44C3-8D51-9ED44863F676}" name="id" totalsRowLabel="요약" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{E272DE11-2CFA-438A-8C30-4093EEBAAD4D}" name="name" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{2CF08806-9622-4698-9F29-63005B4ACF6B}" name="name_en" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{494873D0-DE71-4A7C-A5C1-1CD13F2D633F}" name="type" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{354215F0-D267-44D0-B417-9824FD6469DC}" name="hp" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{B4511A73-E29D-4385-AE5F-8C007E1D956D}" name="atk" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{C37631EF-1FE2-449B-8ADB-3FC65C48BB02}" name="def" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{47878641-5549-4C24-8792-3F626D6AFFF8}" name="image" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{2DFA05EF-9697-418B-B5C7-E4A0E66783E9}" name="sound" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{105408C5-D9C0-44F0-A870-D9BE4782B17F}" name="enemy_info" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}" name="표16" displayName="표16" ref="A1:J9" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}" name="표16" displayName="표16" ref="A1:J9" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:J9" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D11EFD70-6973-4140-97D4-CD2907E8D93F}" name="id" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{96652DA7-C7A3-4D7A-AF4E-3D809758DBDF}" name="name" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{D27CAD10-0AF2-45E2-A350-0DCB9D7368C8}" name="name_en" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{64BCAD89-5438-44B8-8B69-14C0D0BEF66B}" name="type" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{C19525A1-B8C2-4874-A15B-672574DD61B5}" name="currency_t/f" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{A479A586-07FB-4AA2-B0B5-C03AB75D9E36}" name="cost" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{F9281021-C49C-42D1-82CE-05029A330282}" name="atk" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{6C43432D-E0D5-4413-9A53-FB2C421A4757}" name="openLv" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{21EF1B20-EBAC-4C89-96B6-F5772A012BF6}" name="image" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{A6B16ED6-B5B5-411B-806E-9C7E67E71A47}" name="sound" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{D11EFD70-6973-4140-97D4-CD2907E8D93F}" name="id" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{96652DA7-C7A3-4D7A-AF4E-3D809758DBDF}" name="name" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{D27CAD10-0AF2-45E2-A350-0DCB9D7368C8}" name="name_en" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{64BCAD89-5438-44B8-8B69-14C0D0BEF66B}" name="type" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{C19525A1-B8C2-4874-A15B-672574DD61B5}" name="currency_t/f" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{A479A586-07FB-4AA2-B0B5-C03AB75D9E36}" name="cost" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{F9281021-C49C-42D1-82CE-05029A330282}" name="atk" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{6C43432D-E0D5-4413-9A53-FB2C421A4757}" name="openLv" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{21EF1B20-EBAC-4C89-96B6-F5772A012BF6}" name="image" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{A6B16ED6-B5B5-411B-806E-9C7E67E71A47}" name="sound" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}" name="표1_8" displayName="표1_8" ref="B3:D9" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}" name="표1_8" displayName="표1_8" ref="B3:D9" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="B3:D9" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{067AA415-18DF-4E25-B1E4-702E5A434479}" name="몬스터유닛" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C2EAD120-8106-48D6-A4BE-6B50127A292A}" name="공격력" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4EA097C8-2E33-4349-95B8-AF57FD207D06}" name="방어력" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{067AA415-18DF-4E25-B1E4-702E5A434479}" name="몬스터유닛" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C2EAD120-8106-48D6-A4BE-6B50127A292A}" name="공격력" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{4EA097C8-2E33-4349-95B8-AF57FD207D06}" name="방어력" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4918,11 +4918,11 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}" name="표1" displayName="표1" ref="B12:C18" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}" name="표1" displayName="표1" ref="B12:C18" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="B12:C18" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63ACFE6B-8148-4D1A-8EE5-804402BB2ABE}" name="몬스터유닛" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{E32E1503-E62F-4EA7-9DB3-CD6644E25D73}" name="체력" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{63ACFE6B-8148-4D1A-8EE5-804402BB2ABE}" name="몬스터유닛" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E32E1503-E62F-4EA7-9DB3-CD6644E25D73}" name="체력" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5561,13 +5561,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5785,10 +5785,10 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="55"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -5970,15 +5970,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5991,7 +5991,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6063,13 +6063,15 @@
       </c>
       <c r="C2" s="11">
         <f>COUNTA(표14[[#This Row],[enemy_unit1]:[enemy_unit3]])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="11" t="str">
         <f>monster_ref!$B$4</f>
         <v>스켈레톤</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>182</v>
+      </c>
       <c r="F2" s="51"/>
       <c r="G2" s="48">
         <v>0</v>

</xml_diff>

<commit_message>
kmk effect + font
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\만두~\게임 프로젝트\4) 2023.10 ~ 2023.12 인턴 프로젝트\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DABABE8-48B5-4683-97E9-ED41F730A1A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E2B4BB-9869-43FC-A0D3-2BFF543C7768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="1800" windowWidth="23256" windowHeight="12576" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
+    <workbookView xWindow="7788" yWindow="1476" windowWidth="34872" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="222">
   <si>
     <t>stage1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -744,22 +744,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>주술사에 의해 영원한 안식에 들지 못하고 말단 병사로 부려지는 몬스터. 몬스터들 중에 최약체로 꼽힌다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>스톤피스트가 얼음원소와 결합해 탄생한 정예 몬스터. 얼음과 바위가 결합해 더욱 단단한 주먹과 외피를 가진다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>유난히 단단한 바위에서 탄생하는 바위형 몬스터. 온몸을 구성하는 바위 덕분에 방어에 특화되어 있다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>크고 날카로운 낫을 주무기로 삼는 정예 몬스터. 특유의 날렵함을 바탕으로한 강력한 공격 덕분에 보스 바로 다음의 지위를 가진다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>reward-coin</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -872,7 +856,43 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>모든 몬스터들의 위에 군림하는 왕.      파괴자란 이름에 걸맞게 그 검에 닿는 모든 것을 파괴하는 강력한 힘을 가졌다.</t>
+    <t>monsterImage/monster_skelleton</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterImage/monster_boss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterImage/monster_grime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterImage/monster_golem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>monsterImage/monster_stonefeast</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>크고 날카로운 낫을 주무기로 삼는 정예 몬스터. \n특유의 날렵함을 바탕으로한 강력한 공격 덕분에 보스 바로 다음의 지위를 가진다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>주술사에 의해 영원한 안식에 들지 못하고 말단 병사로 부려지는\n몬스터.\n몬스터들 중에 최약체로 꼽힌다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유난히 단단한 바위에서\n탄생하는 바위형 몬스터. \n온몸을 구성하는 바위 덕분에 방어에 특화되어 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 몬스터들의 위에\n군림하는 왕.\n파괴자란 이름에 걸맞게 그 검에 닿는 모든 것을 파괴하는 강력한 힘을\n가졌다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>스톤피스트가 얼음원소와\n결합해 탄생한 정예 몬스터. \n얼음과 바위가 결합해 더욱 단단한 주먹과 외피를 가진다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1438,7 +1458,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1583,9 +1603,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1601,10 +1618,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1616,6 +1633,10 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="68">
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2299,9 +2320,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
@@ -4629,7 +4647,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="몬스터"/>
@@ -4824,21 +4842,21 @@
     <tableColumn id="6" xr3:uid="{822F2BAA-16F4-4BC6-9BCB-01758A14B4CF}" name="enemy_unit3" dataDxfId="50">
       <calculatedColumnFormula>표3[[#This Row],[name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{08FE4F30-2D1A-48D4-B845-F2EF9F32375F}" name="reward_hp" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{09318C06-AB06-4E71-AAD3-53C176D856D4}" name="reward_point" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{DC5BC79E-8C2D-4FB9-BF6E-051A19757C96}" name="reward_coin" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{9ACB5939-E1BD-48F3-8490-09A8DF246598}" name="open_item" dataDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{6988D6FA-4BE7-4E74-B798-7FF44AD473F7}" name="image" dataDxfId="45"/>
-    <tableColumn id="12" xr3:uid="{08CE1504-5F64-4F38-8E02-BA3C4A127ACB}" name="sound" dataDxfId="44"/>
-    <tableColumn id="13" xr3:uid="{16AC2542-0BB8-4573-B0D6-E7FC48FC2FF0}" name="stage_fullname" dataDxfId="43"/>
-    <tableColumn id="14" xr3:uid="{CC2A6C46-331D-4AA2-B4BA-67EC194D8A2F}" name="stage_info" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{08FE4F30-2D1A-48D4-B845-F2EF9F32375F}" name="reward_hp" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{09318C06-AB06-4E71-AAD3-53C176D856D4}" name="reward_point" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{DC5BC79E-8C2D-4FB9-BF6E-051A19757C96}" name="reward_coin" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{9ACB5939-E1BD-48F3-8490-09A8DF246598}" name="open_item" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{6988D6FA-4BE7-4E74-B798-7FF44AD473F7}" name="image" dataDxfId="46"/>
+    <tableColumn id="12" xr3:uid="{08CE1504-5F64-4F38-8E02-BA3C4A127ACB}" name="sound" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{16AC2542-0BB8-4573-B0D6-E7FC48FC2FF0}" name="stage_fullname" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{CC2A6C46-331D-4AA2-B4BA-67EC194D8A2F}" name="stage_info" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}" name="표3" displayName="표3" ref="A1:J7" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}" name="표3" displayName="표3" ref="A1:J7" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A1:J7" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4852,47 +4870,47 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{38E8F74F-24B3-44C3-8D51-9ED44863F676}" name="id" totalsRowLabel="요약" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{E272DE11-2CFA-438A-8C30-4093EEBAAD4D}" name="name" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{2CF08806-9622-4698-9F29-63005B4ACF6B}" name="name_en" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{494873D0-DE71-4A7C-A5C1-1CD13F2D633F}" name="type" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{354215F0-D267-44D0-B417-9824FD6469DC}" name="hp" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{B4511A73-E29D-4385-AE5F-8C007E1D956D}" name="atk" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{C37631EF-1FE2-449B-8ADB-3FC65C48BB02}" name="def" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{47878641-5549-4C24-8792-3F626D6AFFF8}" name="image" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{2DFA05EF-9697-418B-B5C7-E4A0E66783E9}" name="sound" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="12" xr3:uid="{105408C5-D9C0-44F0-A870-D9BE4782B17F}" name="enemy_info" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{38E8F74F-24B3-44C3-8D51-9ED44863F676}" name="id" totalsRowLabel="요약" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{E272DE11-2CFA-438A-8C30-4093EEBAAD4D}" name="name" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{2CF08806-9622-4698-9F29-63005B4ACF6B}" name="name_en" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{494873D0-DE71-4A7C-A5C1-1CD13F2D633F}" name="type" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{354215F0-D267-44D0-B417-9824FD6469DC}" name="hp" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{B4511A73-E29D-4385-AE5F-8C007E1D956D}" name="atk" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{C37631EF-1FE2-449B-8ADB-3FC65C48BB02}" name="def" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{47878641-5549-4C24-8792-3F626D6AFFF8}" name="image" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{2DFA05EF-9697-418B-B5C7-E4A0E66783E9}" name="sound" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{105408C5-D9C0-44F0-A870-D9BE4782B17F}" name="enemy_info" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}" name="표16" displayName="표16" ref="A1:J9" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}" name="표16" displayName="표16" ref="A1:J9" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:J9" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D11EFD70-6973-4140-97D4-CD2907E8D93F}" name="id" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{96652DA7-C7A3-4D7A-AF4E-3D809758DBDF}" name="name" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{D27CAD10-0AF2-45E2-A350-0DCB9D7368C8}" name="name_en" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{64BCAD89-5438-44B8-8B69-14C0D0BEF66B}" name="type" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{C19525A1-B8C2-4874-A15B-672574DD61B5}" name="currency_t/f" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{A479A586-07FB-4AA2-B0B5-C03AB75D9E36}" name="cost" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{F9281021-C49C-42D1-82CE-05029A330282}" name="atk" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{6C43432D-E0D5-4413-9A53-FB2C421A4757}" name="openLv" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{21EF1B20-EBAC-4C89-96B6-F5772A012BF6}" name="image" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{A6B16ED6-B5B5-411B-806E-9C7E67E71A47}" name="sound" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{D11EFD70-6973-4140-97D4-CD2907E8D93F}" name="id" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{96652DA7-C7A3-4D7A-AF4E-3D809758DBDF}" name="name" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{D27CAD10-0AF2-45E2-A350-0DCB9D7368C8}" name="name_en" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{64BCAD89-5438-44B8-8B69-14C0D0BEF66B}" name="type" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{C19525A1-B8C2-4874-A15B-672574DD61B5}" name="currency_t/f" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{A479A586-07FB-4AA2-B0B5-C03AB75D9E36}" name="cost" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{F9281021-C49C-42D1-82CE-05029A330282}" name="atk" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{6C43432D-E0D5-4413-9A53-FB2C421A4757}" name="openLv" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{21EF1B20-EBAC-4C89-96B6-F5772A012BF6}" name="image" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{A6B16ED6-B5B5-411B-806E-9C7E67E71A47}" name="sound" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}" name="표1_8" displayName="표1_8" ref="B3:D9" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}" name="표1_8" displayName="표1_8" ref="B3:D9" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B3:D9" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{067AA415-18DF-4E25-B1E4-702E5A434479}" name="몬스터유닛" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{C2EAD120-8106-48D6-A4BE-6B50127A292A}" name="공격력" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{4EA097C8-2E33-4349-95B8-AF57FD207D06}" name="방어력" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{067AA415-18DF-4E25-B1E4-702E5A434479}" name="몬스터유닛" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C2EAD120-8106-48D6-A4BE-6B50127A292A}" name="공격력" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4EA097C8-2E33-4349-95B8-AF57FD207D06}" name="방어력" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4918,11 +4936,11 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}" name="표1" displayName="표1" ref="B12:C18" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}" name="표1" displayName="표1" ref="B12:C18" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="B12:C18" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63ACFE6B-8148-4D1A-8EE5-804402BB2ABE}" name="몬스터유닛" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{E32E1503-E62F-4EA7-9DB3-CD6644E25D73}" name="체력" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{63ACFE6B-8148-4D1A-8EE5-804402BB2ABE}" name="몬스터유닛" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E32E1503-E62F-4EA7-9DB3-CD6644E25D73}" name="체력" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5262,21 +5280,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="48" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:5" s="11" customFormat="1" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B3" s="50">
+      <c r="B3" s="49">
         <v>1</v>
       </c>
       <c r="C3" s="28" t="s">
@@ -5290,7 +5308,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B4" s="50">
+      <c r="B4" s="49">
         <v>2</v>
       </c>
       <c r="C4" s="28" t="s">
@@ -5304,7 +5322,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B5" s="50">
+      <c r="B5" s="49">
         <v>3</v>
       </c>
       <c r="C5" s="28" t="s">
@@ -5318,7 +5336,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B6" s="50">
+      <c r="B6" s="49">
         <v>4</v>
       </c>
       <c r="C6" s="28" t="s">
@@ -5332,7 +5350,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B7" s="50">
+      <c r="B7" s="49">
         <v>5</v>
       </c>
       <c r="C7" s="28" t="s">
@@ -5346,7 +5364,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B8" s="50">
+      <c r="B8" s="49">
         <v>6</v>
       </c>
       <c r="C8" s="28" t="s">
@@ -5360,7 +5378,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B9" s="50">
+      <c r="B9" s="49">
         <v>7</v>
       </c>
       <c r="C9" s="28" t="s">
@@ -5374,7 +5392,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B10" s="50">
+      <c r="B10" s="49">
         <v>8</v>
       </c>
       <c r="C10" s="28" t="s">
@@ -5388,7 +5406,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B11" s="50">
+      <c r="B11" s="49">
         <v>9</v>
       </c>
       <c r="C11" s="28" t="s">
@@ -5402,7 +5420,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B12" s="50">
+      <c r="B12" s="49">
         <v>10</v>
       </c>
       <c r="C12" s="28" t="s">
@@ -5416,7 +5434,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B13" s="50">
+      <c r="B13" s="49">
         <v>11</v>
       </c>
       <c r="C13" s="28" t="s">
@@ -5430,7 +5448,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B14" s="50">
+      <c r="B14" s="49">
         <v>12</v>
       </c>
       <c r="C14" s="28" t="s">
@@ -5444,7 +5462,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B15" s="50">
+      <c r="B15" s="49">
         <v>13</v>
       </c>
       <c r="C15" s="28" t="s">
@@ -5458,21 +5476,21 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B16" s="50">
+      <c r="B16" s="49">
         <v>14</v>
       </c>
       <c r="C16" s="28" t="s">
         <v>126</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B17" s="50">
+      <c r="B17" s="49">
         <v>15</v>
       </c>
       <c r="C17" s="28" t="s">
@@ -5486,7 +5504,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B18" s="50">
+      <c r="B18" s="49">
         <v>16</v>
       </c>
       <c r="C18" s="28" t="s">
@@ -5500,7 +5518,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B19" s="50">
+      <c r="B19" s="49">
         <v>17</v>
       </c>
       <c r="C19" s="28" t="s">
@@ -5514,7 +5532,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
-      <c r="B20" s="50">
+      <c r="B20" s="49">
         <v>18</v>
       </c>
       <c r="C20" s="28" t="s">
@@ -5561,30 +5579,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="53"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
@@ -5693,10 +5711,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="18"/>
       <c r="E10" s="14" t="s">
         <v>16</v>
@@ -5750,10 +5768,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="53"/>
+      <c r="F13" s="52"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5802,10 +5820,10 @@
         <v>35</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="53"/>
+      <c r="F17" s="52"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -5843,10 +5861,10 @@
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="18"/>
       <c r="E20" s="14" t="s">
         <v>40</v>
@@ -5970,15 +5988,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5991,7 +6009,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6001,11 +6019,12 @@
     <col min="3" max="3" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.69921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.69921875" customWidth="1"/>
     <col min="13" max="13" width="15.8984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="147.3984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -6048,10 +6067,10 @@
         <v>139</v>
       </c>
       <c r="M1" s="47" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="N1" s="47" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.4">
@@ -6072,8 +6091,8 @@
       <c r="E2" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="F2" s="51"/>
-      <c r="G2" s="48">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50">
         <v>0</v>
       </c>
       <c r="H2" s="11">
@@ -6086,10 +6105,10 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
@@ -6111,8 +6130,8 @@
         <f>표3[[#This Row],[name]]</f>
         <v>스톤피스트</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="48">
+      <c r="F3" s="50"/>
+      <c r="G3" s="50">
         <v>2</v>
       </c>
       <c r="H3" s="11">
@@ -6122,15 +6141,15 @@
         <v>110</v>
       </c>
       <c r="J3" s="46" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="N3" s="52" t="s">
         <v>211</v>
+      </c>
+      <c r="N3" s="51" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
@@ -6149,8 +6168,8 @@
         <v>아이스골렘</v>
       </c>
       <c r="E4" s="11"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="48">
+      <c r="F4" s="50"/>
+      <c r="G4" s="50">
         <v>0</v>
       </c>
       <c r="H4" s="11">
@@ -6165,10 +6184,10 @@
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
@@ -6190,8 +6209,8 @@
         <f>표3[[#This Row],[name]]</f>
         <v>그림 리퍼</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="48">
+      <c r="F5" s="50"/>
+      <c r="G5" s="50">
         <v>2</v>
       </c>
       <c r="H5" s="11">
@@ -6206,10 +6225,10 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
@@ -6231,11 +6250,11 @@
         <f>monster_Data!B3</f>
         <v>스톤피스트</v>
       </c>
-      <c r="F6" s="51" t="str">
+      <c r="F6" s="50" t="str">
         <f>표3[[#This Row],[name]]</f>
         <v>파괴자 모로스</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="50">
         <v>0</v>
       </c>
       <c r="H6" s="11">
@@ -6248,10 +6267,10 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="19.2" x14ac:dyDescent="0.4">
@@ -6281,7 +6300,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6292,7 +6311,7 @@
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.19921875" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="131.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="117.19921875" bestFit="1" customWidth="1"/>
@@ -6346,7 +6365,7 @@
         <v>스켈레톤</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D2" s="28" t="str">
         <f>ID_code!I7</f>
@@ -6364,10 +6383,12 @@
         <f>VLOOKUP(표3[[#This Row],[name]],표1_8[#All],3,)</f>
         <v>10</v>
       </c>
-      <c r="H2" s="18"/>
+      <c r="H2" s="18" t="s">
+        <v>212</v>
+      </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6379,7 +6400,7 @@
         <v>스톤피스트</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>114</v>
@@ -6396,10 +6417,12 @@
         <f>VLOOKUP(표3[[#This Row],[name]],표1_8[#All],3,)</f>
         <v>13</v>
       </c>
-      <c r="H3" s="18"/>
+      <c r="H3" s="18" t="s">
+        <v>216</v>
+      </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18" t="s">
-        <v>186</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6411,7 +6434,7 @@
         <v>아이스골렘</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>114</v>
@@ -6428,10 +6451,12 @@
         <f>VLOOKUP(표3[[#This Row],[name]],표1_8[#All],3,)</f>
         <v>20</v>
       </c>
-      <c r="H4" s="18"/>
+      <c r="H4" s="18" t="s">
+        <v>215</v>
+      </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6443,7 +6468,7 @@
         <v>그림 리퍼</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D5" s="28" t="s">
         <v>114</v>
@@ -6460,10 +6485,12 @@
         <f>VLOOKUP(표3[[#This Row],[name]],표1_8[#All],3,)</f>
         <v>20</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>214</v>
+      </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6475,7 +6502,7 @@
         <v>파괴자 모로스</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>114</v>
@@ -6492,10 +6519,12 @@
         <f>VLOOKUP(표3[[#This Row],[name]],표1_8[#All],3,)</f>
         <v>30</v>
       </c>
-      <c r="H6" s="18"/>
+      <c r="H6" s="18" t="s">
+        <v>213</v>
+      </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6507,7 +6536,7 @@
         <v>파괴자 모로스</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>114</v>
@@ -6524,10 +6553,12 @@
         <f>VLOOKUP(표3[[#This Row],[name]],표1_8[#All],3,)</f>
         <v>30</v>
       </c>
-      <c r="H7" s="18"/>
+      <c r="H7" s="18" t="s">
+        <v>213</v>
+      </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -6624,7 +6655,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D3" s="28" t="str">
         <f>ID_code!I8</f>
@@ -6729,10 +6760,10 @@
         <v>3521</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D7" s="28" t="str">
         <f>ID_code!I9</f>
@@ -6758,10 +6789,10 @@
         <v>3522</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D8" s="28" t="str">
         <f>ID_code!I9</f>
@@ -6787,10 +6818,10 @@
         <v>3523</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D9" s="28" t="str">
         <f>ID_code!I9</f>
@@ -6905,25 +6936,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="G2" s="56" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="G2" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B3" s="21" t="s">
@@ -7081,7 +7112,7 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B7" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
@@ -7120,7 +7151,7 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B8" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C8" s="1">
         <v>30</v>
@@ -7148,10 +7179,10 @@
       </c>
     </row>
     <row r="11" spans="2:17" ht="21" x14ac:dyDescent="0.4">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="56"/>
+      <c r="C11" s="55"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B12" s="21" t="s">

</xml_diff>

<commit_message>
kmk - UI Change
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E2B4BB-9869-43FC-A0D3-2BFF543C7768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DB25D0-CAB0-4DF6-9018-48725DBA1F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7788" yWindow="1476" windowWidth="34872" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
+    <workbookView xWindow="8988" yWindow="1344" windowWidth="34872" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="222">
   <si>
     <t>stage1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1618,10 +1618,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1633,10 +1633,6 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="68">
-    <dxf>
-      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2319,6 +2315,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4842,21 +4842,21 @@
     <tableColumn id="6" xr3:uid="{822F2BAA-16F4-4BC6-9BCB-01758A14B4CF}" name="enemy_unit3" dataDxfId="50">
       <calculatedColumnFormula>표3[[#This Row],[name]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{08FE4F30-2D1A-48D4-B845-F2EF9F32375F}" name="reward_hp" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{09318C06-AB06-4E71-AAD3-53C176D856D4}" name="reward_point" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{DC5BC79E-8C2D-4FB9-BF6E-051A19757C96}" name="reward_coin" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{9ACB5939-E1BD-48F3-8490-09A8DF246598}" name="open_item" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{6988D6FA-4BE7-4E74-B798-7FF44AD473F7}" name="image" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{08CE1504-5F64-4F38-8E02-BA3C4A127ACB}" name="sound" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{16AC2542-0BB8-4573-B0D6-E7FC48FC2FF0}" name="stage_fullname" dataDxfId="44"/>
-    <tableColumn id="14" xr3:uid="{CC2A6C46-331D-4AA2-B4BA-67EC194D8A2F}" name="stage_info" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{08FE4F30-2D1A-48D4-B845-F2EF9F32375F}" name="reward_hp" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{09318C06-AB06-4E71-AAD3-53C176D856D4}" name="reward_point" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{DC5BC79E-8C2D-4FB9-BF6E-051A19757C96}" name="reward_coin" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{9ACB5939-E1BD-48F3-8490-09A8DF246598}" name="open_item" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{6988D6FA-4BE7-4E74-B798-7FF44AD473F7}" name="image" dataDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{08CE1504-5F64-4F38-8E02-BA3C4A127ACB}" name="sound" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{16AC2542-0BB8-4573-B0D6-E7FC48FC2FF0}" name="stage_fullname" dataDxfId="43"/>
+    <tableColumn id="14" xr3:uid="{CC2A6C46-331D-4AA2-B4BA-67EC194D8A2F}" name="stage_info" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}" name="표3" displayName="표3" ref="A1:J7" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}" name="표3" displayName="표3" ref="A1:J7" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A1:J7" xr:uid="{E2E5F455-C004-4A3D-BF7D-328FF88528E7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4870,47 +4870,47 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{38E8F74F-24B3-44C3-8D51-9ED44863F676}" name="id" totalsRowLabel="요약" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{E272DE11-2CFA-438A-8C30-4093EEBAAD4D}" name="name" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{2CF08806-9622-4698-9F29-63005B4ACF6B}" name="name_en" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{494873D0-DE71-4A7C-A5C1-1CD13F2D633F}" name="type" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{354215F0-D267-44D0-B417-9824FD6469DC}" name="hp" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{B4511A73-E29D-4385-AE5F-8C007E1D956D}" name="atk" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{C37631EF-1FE2-449B-8ADB-3FC65C48BB02}" name="def" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{47878641-5549-4C24-8792-3F626D6AFFF8}" name="image" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{2DFA05EF-9697-418B-B5C7-E4A0E66783E9}" name="sound" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{105408C5-D9C0-44F0-A870-D9BE4782B17F}" name="enemy_info" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{38E8F74F-24B3-44C3-8D51-9ED44863F676}" name="id" totalsRowLabel="요약" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{E272DE11-2CFA-438A-8C30-4093EEBAAD4D}" name="name" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{2CF08806-9622-4698-9F29-63005B4ACF6B}" name="name_en" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{494873D0-DE71-4A7C-A5C1-1CD13F2D633F}" name="type" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{354215F0-D267-44D0-B417-9824FD6469DC}" name="hp" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{B4511A73-E29D-4385-AE5F-8C007E1D956D}" name="atk" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{C37631EF-1FE2-449B-8ADB-3FC65C48BB02}" name="def" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{47878641-5549-4C24-8792-3F626D6AFFF8}" name="image" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{2DFA05EF-9697-418B-B5C7-E4A0E66783E9}" name="sound" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{105408C5-D9C0-44F0-A870-D9BE4782B17F}" name="enemy_info" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}" name="표16" displayName="표16" ref="A1:J9" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}" name="표16" displayName="표16" ref="A1:J9" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A1:J9" xr:uid="{A32CF929-9BAE-487E-AA59-E59A097DB6ED}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{D11EFD70-6973-4140-97D4-CD2907E8D93F}" name="id" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{96652DA7-C7A3-4D7A-AF4E-3D809758DBDF}" name="name" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{D27CAD10-0AF2-45E2-A350-0DCB9D7368C8}" name="name_en" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{64BCAD89-5438-44B8-8B69-14C0D0BEF66B}" name="type" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{C19525A1-B8C2-4874-A15B-672574DD61B5}" name="currency_t/f" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{A479A586-07FB-4AA2-B0B5-C03AB75D9E36}" name="cost" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{F9281021-C49C-42D1-82CE-05029A330282}" name="atk" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{6C43432D-E0D5-4413-9A53-FB2C421A4757}" name="openLv" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{21EF1B20-EBAC-4C89-96B6-F5772A012BF6}" name="image" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{A6B16ED6-B5B5-411B-806E-9C7E67E71A47}" name="sound" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{D11EFD70-6973-4140-97D4-CD2907E8D93F}" name="id" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{96652DA7-C7A3-4D7A-AF4E-3D809758DBDF}" name="name" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{D27CAD10-0AF2-45E2-A350-0DCB9D7368C8}" name="name_en" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{64BCAD89-5438-44B8-8B69-14C0D0BEF66B}" name="type" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{C19525A1-B8C2-4874-A15B-672574DD61B5}" name="currency_t/f" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{A479A586-07FB-4AA2-B0B5-C03AB75D9E36}" name="cost" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{F9281021-C49C-42D1-82CE-05029A330282}" name="atk" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{6C43432D-E0D5-4413-9A53-FB2C421A4757}" name="openLv" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{21EF1B20-EBAC-4C89-96B6-F5772A012BF6}" name="image" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{A6B16ED6-B5B5-411B-806E-9C7E67E71A47}" name="sound" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}" name="표1_8" displayName="표1_8" ref="B3:D9" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}" name="표1_8" displayName="표1_8" ref="B3:D9" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="B3:D9" xr:uid="{DCDA4F24-5C72-4BAC-95D6-FA90FEDAFDFB}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{067AA415-18DF-4E25-B1E4-702E5A434479}" name="몬스터유닛" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C2EAD120-8106-48D6-A4BE-6B50127A292A}" name="공격력" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{4EA097C8-2E33-4349-95B8-AF57FD207D06}" name="방어력" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{067AA415-18DF-4E25-B1E4-702E5A434479}" name="몬스터유닛" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C2EAD120-8106-48D6-A4BE-6B50127A292A}" name="공격력" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{4EA097C8-2E33-4349-95B8-AF57FD207D06}" name="방어력" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4936,11 +4936,11 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}" name="표1" displayName="표1" ref="B12:C18" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}" name="표1" displayName="표1" ref="B12:C18" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="B12:C18" xr:uid="{2AA2D02D-1F9D-4FC7-B9FA-62D4EA30C842}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63ACFE6B-8148-4D1A-8EE5-804402BB2ABE}" name="몬스터유닛" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{E32E1503-E62F-4EA7-9DB3-CD6644E25D73}" name="체력" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{63ACFE6B-8148-4D1A-8EE5-804402BB2ABE}" name="몬스터유닛" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E32E1503-E62F-4EA7-9DB3-CD6644E25D73}" name="체력" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="표 스타일 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5579,13 +5579,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5803,10 +5803,10 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -5988,15 +5988,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6009,7 +6009,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6082,15 +6082,13 @@
       </c>
       <c r="C2" s="11">
         <f>COUNTA(표14[[#This Row],[enemy_unit1]:[enemy_unit3]])</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="11" t="str">
         <f>monster_ref!$B$4</f>
         <v>스켈레톤</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>182</v>
-      </c>
+      <c r="E2" s="11"/>
       <c r="F2" s="50"/>
       <c r="G2" s="50">
         <v>0</v>

</xml_diff>

<commit_message>
kmk - sfx end
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68339E66-A636-4ECA-9E23-69B9CD05E703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9AAB35-F1AA-417D-A1C4-3839649B78DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1308" yWindow="1416" windowWidth="24336" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
@@ -1615,10 +1615,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5579,30 +5579,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="53"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
@@ -5711,10 +5711,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="18"/>
       <c r="E10" s="14" t="s">
         <v>16</v>
@@ -5768,10 +5768,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="53"/>
+      <c r="F13" s="52"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5820,10 +5820,10 @@
         <v>35</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="53"/>
+      <c r="F17" s="52"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -5861,10 +5861,10 @@
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="18"/>
       <c r="E20" s="14" t="s">
         <v>40</v>
@@ -5988,15 +5988,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6009,7 +6009,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
kmk-bgm add and bug fix
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3190E6-AA0D-4EC1-B1AA-7216BFD27C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0F241D-8D08-4CAA-A96B-A641293E7C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1308" yWindow="1416" windowWidth="24336" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
+    <workbookView xWindow="1308" yWindow="1416" windowWidth="35160" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="222">
   <si>
     <t>stage1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -832,26 +832,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>얼떨결에 용사의 길을 걷게된 당신. 두려운 마음이 크지만 용기를 내 여정을 떠나기로 결심합니다. 결심한지 얼마 지나지 않아 몬스터를 마주치게 되는데..</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">첫 전투에서 승리하고 성을 향해 다시 나아갑니다. 하지만 성까지 가는 길에는 수많은 몬스터들이 당신을 기다리고 있었습니다. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>겨우 도착한 목적지에 보이는 것은 굳게 닫힌 문과 이를 지키는 강력한 몬스터입니다. 이전과 다른 분위기에 긴장되지만 왠지 이길 수 있을 것만 같다는 생각이 듭니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>무사히 성 안에 들어온 당신. 성 안은 어둡고 적막만이 가득합니다. 빨리 전쟁을 끝내기 위해 보스를 찾아보지만 그 길목에서 마주친건 또다른 몬스터 무리였습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">이제는 정말 모든 것을 끝낼 시간입니다. 주사위와 함께 강해진 당신은 보스를 마주해도 더 이상 두렵지 않습니다. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>힘겨운 전진</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -880,19 +860,39 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>주술사에 의해 영원한 안식에 들지 못하고 말단 병사로 부려지는\n몬스터.\n몬스터들 중에 최약체로 꼽힌다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>유난히 단단한 바위에서\n탄생하는 바위형 몬스터. \n온몸을 구성하는 바위 덕분에 방어에 특화되어 있다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>모든 몬스터들의 위에\n군림하는 왕.\n파괴자란 이름에 걸맞게 그 검에 닿는 모든 것을 파괴하는 강력한 힘을\n가졌다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>스톤피스트가 얼음원소와\n결합해 탄생한 정예 몬스터. \n얼음과 바위가 결합해 더욱 단단한 주먹과 외피를 가진다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\n주술사에 의해 영원한 안식에 들지\n못하고 말단 병사로 부려지는 몬스터.\n몬스터들 중에 최약체로 꼽힌다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\n유난히 단단한 바위에서 탄생하는\n바위형 몬스터. \n온몸을 구성하는 바위 덕분에 방어에\n특화되어 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>얼떨결에 용사의 길을 걷게된 당신.\n두려운 마음이 크지만 용기를 내 여정을 떠나기로 결심합니다.\n결심한지 얼마 지나지 않아 몬스터를 마주치게 되는데..</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>무사히 성 안에 들어온 당신.\n성 안은 어둡고 적막만이 가득합니다.\n빨리 전쟁을 끝내기 위해 보스를 찾아보지만 그 길목에서 마주친건 또다른 몬스터 무리였습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">이제는 정말 모든 것을 끝낼 시간입니다.\n주사위와 함께 강해진 당신은 보스를 마주해도 더 이상 두렵지 않습니다. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>겨우 도착한 목적지에 보이는 것은 굳게 닫힌 문과 이를 지키는 강력한 몬스터입니다.\n이전과 다른 분위기에 긴장되지만 왠지 이길 수 있을 것만 같다는 생각이 듭니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">첫 전투에서 승리하고 성을 향해 다시 나아갑니다.\n하지만 성까지 가는 길에는 수많은 몬스터들이 당신을 기다리고 있었습니다. </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1615,10 +1615,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5579,30 +5579,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="53"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="53"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
@@ -5711,10 +5711,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="18"/>
       <c r="E10" s="14" t="s">
         <v>16</v>
@@ -5768,10 +5768,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="53"/>
+      <c r="F13" s="52"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5820,10 +5820,10 @@
         <v>35</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="53"/>
+      <c r="F17" s="52"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -5861,10 +5861,10 @@
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="18"/>
       <c r="E20" s="14" t="s">
         <v>40</v>
@@ -5988,15 +5988,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6008,8 +6008,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6084,9 +6084,8 @@
         <f>COUNTA(표14[[#This Row],[enemy_unit1]:[enemy_unit3]])</f>
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="str">
-        <f>monster_ref!$B$4</f>
-        <v>스켈레톤</v>
+      <c r="D2" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="50"/>
@@ -6106,7 +6105,7 @@
         <v>201</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.4">
@@ -6143,10 +6142,10 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="N3" s="51" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.4">
@@ -6183,7 +6182,7 @@
         <v>202</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.4">
@@ -6223,7 +6222,7 @@
         <v>204</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.4">
@@ -6265,7 +6264,7 @@
         <v>205</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="19.2" x14ac:dyDescent="0.4">
@@ -6295,7 +6294,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6379,11 +6378,11 @@
         <v>10</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6413,11 +6412,11 @@
         <v>13</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6447,11 +6446,11 @@
         <v>20</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6481,11 +6480,11 @@
         <v>20</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6515,11 +6514,11 @@
         <v>30</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
@@ -6549,11 +6548,11 @@
         <v>30</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kmk dice + boss 15 round
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0F241D-8D08-4CAA-A96B-A641293E7C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921238CF-D88F-46E6-9ED1-766130FEF6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1308" yWindow="1416" windowWidth="35160" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="222">
   <si>
     <t>stage1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1618,10 +1618,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5579,13 +5579,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
@@ -5803,10 +5803,10 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -5988,15 +5988,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6008,8 +6008,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6119,9 +6119,8 @@
         <f>COUNTA(표14[[#This Row],[enemy_unit1]:[enemy_unit3]])</f>
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="str">
-        <f>monster_ref!B4</f>
-        <v>스켈레톤</v>
+      <c r="D3" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>180</v>
@@ -6196,9 +6195,8 @@
         <f>COUNTA(표14[[#This Row],[enemy_unit1]:[enemy_unit3]])</f>
         <v>2</v>
       </c>
-      <c r="D5" s="11" t="str">
-        <f>monster_Data!B2</f>
-        <v>스켈레톤</v>
+      <c r="D5" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>180</v>
@@ -6236,9 +6234,8 @@
         <f>COUNTA(표14[[#This Row],[enemy_unit1]:[enemy_unit3]])</f>
         <v>3</v>
       </c>
-      <c r="D6" s="11" t="str">
-        <f>monster_Data!B2</f>
-        <v>스켈레톤</v>
+      <c r="D6" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="E6" s="11" t="str">
         <f>monster_Data!B2</f>

</xml_diff>

<commit_message>
kmk - bug fix
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\kmk\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16524782-F161-4DB7-AC03-3DC838B6D268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C26EE5A-8C39-490F-B97E-961B5638D5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="2160" windowWidth="36150" windowHeight="18210" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
+    <workbookView xWindow="1308" yWindow="1416" windowWidth="35160" windowHeight="16284" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="8" r:id="rId1"/>
@@ -1458,7 +1458,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1615,19 +1615,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5273,16 +5270,16 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.875" customWidth="1"/>
-    <col min="2" max="2" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.8984375" customWidth="1"/>
+    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="78" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="48" t="s">
         <v>35</v>
       </c>
@@ -5296,7 +5293,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="2:5" s="11" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" s="11" customFormat="1" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B3" s="49">
         <v>1</v>
       </c>
@@ -5310,7 +5307,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B4" s="49">
         <v>2</v>
       </c>
@@ -5324,7 +5321,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B5" s="49">
         <v>3</v>
       </c>
@@ -5338,7 +5335,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B6" s="49">
         <v>4</v>
       </c>
@@ -5352,7 +5349,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B7" s="49">
         <v>5</v>
       </c>
@@ -5366,7 +5363,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B8" s="49">
         <v>6</v>
       </c>
@@ -5380,7 +5377,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B9" s="49">
         <v>7</v>
       </c>
@@ -5394,7 +5391,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B10" s="49">
         <v>8</v>
       </c>
@@ -5408,7 +5405,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B11" s="49">
         <v>9</v>
       </c>
@@ -5422,7 +5419,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B12" s="49">
         <v>10</v>
       </c>
@@ -5436,7 +5433,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B13" s="49">
         <v>11</v>
       </c>
@@ -5450,7 +5447,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B14" s="49">
         <v>12</v>
       </c>
@@ -5464,7 +5461,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B15" s="49">
         <v>13</v>
       </c>
@@ -5478,7 +5475,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B16" s="49">
         <v>14</v>
       </c>
@@ -5492,7 +5489,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B17" s="49">
         <v>15</v>
       </c>
@@ -5506,7 +5503,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B18" s="49">
         <v>16</v>
       </c>
@@ -5520,7 +5517,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B19" s="49">
         <v>17</v>
       </c>
@@ -5534,7 +5531,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B20" s="49">
         <v>18</v>
       </c>
@@ -5548,7 +5545,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B22" s="28"/>
       <c r="C22" s="28"/>
     </row>
@@ -5571,43 +5568,43 @@
       <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.25" customWidth="1"/>
-    <col min="5" max="5" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.59765625" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.19921875" customWidth="1"/>
+    <col min="5" max="5" width="13.69921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.5" customWidth="1"/>
-    <col min="8" max="8" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
+    <row r="2" spans="2:9" ht="25.2" x14ac:dyDescent="0.4">
+      <c r="B2" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-    </row>
-    <row r="3" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="53" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+    </row>
+    <row r="3" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="53"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="53"/>
-    </row>
-    <row r="5" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="52"/>
+    </row>
+    <row r="5" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="12" t="s">
         <v>32</v>
       </c>
@@ -5629,7 +5626,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B6" s="14" t="s">
         <v>33</v>
       </c>
@@ -5651,7 +5648,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
@@ -5673,7 +5670,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="16" t="s">
         <v>34</v>
       </c>
@@ -5695,7 +5692,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -5713,11 +5710,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="53" t="s">
+    <row r="10" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="18"/>
       <c r="E10" s="14" t="s">
         <v>16</v>
@@ -5733,7 +5730,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B11" s="36" t="s">
         <v>29</v>
       </c>
@@ -5751,7 +5748,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
         <v>27</v>
       </c>
@@ -5763,7 +5760,7 @@
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="14" t="s">
         <v>30</v>
       </c>
@@ -5771,13 +5768,13 @@
         <v>2</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="53"/>
+      <c r="F13" s="52"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="16" t="s">
         <v>31</v>
       </c>
@@ -5793,7 +5790,7 @@
       </c>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -5805,7 +5802,7 @@
       </c>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="54" t="s">
         <v>58</v>
       </c>
@@ -5815,7 +5812,7 @@
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
@@ -5823,15 +5820,15 @@
         <v>35</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="53"/>
+      <c r="F17" s="52"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="36" t="s">
         <v>59</v>
       </c>
@@ -5849,7 +5846,7 @@
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -5863,11 +5860,11 @@
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="53" t="s">
+    <row r="20" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="18"/>
       <c r="E20" s="14" t="s">
         <v>40</v>
@@ -5879,7 +5876,7 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="36" t="s">
         <v>29</v>
       </c>
@@ -5897,7 +5894,7 @@
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
     </row>
-    <row r="22" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B22" s="12" t="s">
         <v>36</v>
       </c>
@@ -5915,7 +5912,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B23" s="14" t="s">
         <v>37</v>
       </c>
@@ -5933,7 +5930,7 @@
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="16" t="s">
         <v>38</v>
       </c>
@@ -5951,7 +5948,7 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
@@ -5965,7 +5962,7 @@
       <c r="H25" s="18"/>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -5979,7 +5976,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="2:9" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
@@ -5991,15 +5988,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6012,27 +6009,27 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.69921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.75" customWidth="1"/>
-    <col min="13" max="13" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="147.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.69921875" customWidth="1"/>
+    <col min="13" max="13" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="147.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>131</v>
       </c>
@@ -6076,7 +6073,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -6111,7 +6108,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -6126,7 +6123,7 @@
         <v>180</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F3" s="50"/>
       <c r="G3" s="50">
@@ -6150,7 +6147,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -6162,7 +6159,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="50"/>
@@ -6187,7 +6184,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -6202,7 +6199,7 @@
         <v>180</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F5" s="50"/>
       <c r="G5" s="50">
@@ -6226,7 +6223,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -6241,10 +6238,10 @@
         <v>180</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="G6" s="50">
         <v>0</v>
@@ -6252,7 +6249,7 @@
       <c r="H6" s="11">
         <v>4</v>
       </c>
-      <c r="I6" s="56">
+      <c r="I6" s="11">
         <v>200</v>
       </c>
       <c r="J6" s="46"/>
@@ -6265,13 +6262,13 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="19.2" x14ac:dyDescent="0.4">
       <c r="I10" s="45"/>
     </row>
-    <row r="11" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="19.2" x14ac:dyDescent="0.4">
       <c r="I11" s="45"/>
     </row>
-    <row r="12" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="19.2" x14ac:dyDescent="0.4">
       <c r="I12" s="45"/>
     </row>
   </sheetData>
@@ -6296,28 +6293,28 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.25" customWidth="1"/>
+    <col min="5" max="5" width="11.19921875" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="131.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="117.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.125" customWidth="1"/>
+    <col min="11" max="11" width="117.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.09765625" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="15.875" customWidth="1"/>
+    <col min="16" max="16" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="15.8984375" customWidth="1"/>
     <col min="21" max="21" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
         <v>106</v>
       </c>
@@ -6349,7 +6346,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A2" s="18">
         <v>2110</v>
       </c>
@@ -6384,7 +6381,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A3" s="18">
         <v>2111</v>
       </c>
@@ -6418,7 +6415,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A4" s="18">
         <v>2212</v>
       </c>
@@ -6452,7 +6449,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A5" s="18">
         <v>2213</v>
       </c>
@@ -6486,7 +6483,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A6" s="18">
         <v>2314</v>
       </c>
@@ -6520,7 +6517,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A7" s="18">
         <v>2315</v>
       </c>
@@ -6572,20 +6569,20 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="6" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3984375" customWidth="1"/>
+    <col min="5" max="6" width="16.8984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.25" customWidth="1"/>
+    <col min="9" max="9" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
         <v>57</v>
       </c>
@@ -6617,7 +6614,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A2" s="28">
         <v>3616</v>
       </c>
@@ -6640,7 +6637,7 @@
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A3" s="28">
         <v>3417</v>
       </c>
@@ -6667,7 +6664,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A4" s="28">
         <v>3418</v>
       </c>
@@ -6694,7 +6691,7 @@
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A5" s="28">
         <v>3419</v>
       </c>
@@ -6721,7 +6718,7 @@
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A6" s="28">
         <v>3420</v>
       </c>
@@ -6748,7 +6745,7 @@
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
     </row>
-    <row r="7" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A7" s="28">
         <v>3521</v>
       </c>
@@ -6777,7 +6774,7 @@
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
     </row>
-    <row r="8" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A8" s="28">
         <v>3522</v>
       </c>
@@ -6806,7 +6803,7 @@
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="A9" s="28">
         <v>3523</v>
       </c>
@@ -6835,7 +6832,7 @@
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
     </row>
-    <row r="11" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -6845,7 +6842,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="30"/>
       <c r="C12" s="43"/>
       <c r="D12" s="43"/>
@@ -6855,37 +6852,37 @@
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B13" s="31"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
     </row>
-    <row r="14" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
     </row>
-    <row r="18" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
     </row>
-    <row r="19" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -6908,27 +6905,27 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.125" customWidth="1"/>
-    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" customWidth="1"/>
-    <col min="9" max="9" width="15.75" customWidth="1"/>
-    <col min="10" max="10" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.09765625" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.3984375" customWidth="1"/>
+    <col min="9" max="9" width="15.69921875" customWidth="1"/>
+    <col min="10" max="10" width="26.69921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="15.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="55" t="s">
         <v>80</v>
       </c>
@@ -6949,7 +6946,7 @@
       <c r="P2" s="55"/>
       <c r="Q2" s="55"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B3" s="21" t="s">
         <v>119</v>
       </c>
@@ -6993,7 +6990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B4" s="5" t="s">
         <v>180</v>
       </c>
@@ -7029,7 +7026,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B5" s="5" t="s">
         <v>182</v>
       </c>
@@ -7067,7 +7064,7 @@
       <c r="O5" s="24"/>
       <c r="P5" s="24"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>181</v>
       </c>
@@ -7103,7 +7100,7 @@
       <c r="O6" s="24"/>
       <c r="P6" s="24"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B7" s="5" t="s">
         <v>185</v>
       </c>
@@ -7142,7 +7139,7 @@
       <c r="O7" s="24"/>
       <c r="P7" s="24"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B8" s="5" t="s">
         <v>197</v>
       </c>
@@ -7156,7 +7153,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B9" s="25" t="str">
         <f>B8</f>
         <v>파괴자 모로스</v>
@@ -7171,13 +7168,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" ht="21" x14ac:dyDescent="0.4">
       <c r="B11" s="55" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="55"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B12" s="21" t="s">
         <v>119</v>
       </c>
@@ -7185,7 +7182,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B13" s="5" t="s">
         <v>180</v>
       </c>
@@ -7193,7 +7190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
         <v>182</v>
       </c>
@@ -7201,7 +7198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B15" s="5" t="s">
         <v>181</v>
       </c>
@@ -7209,7 +7206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B16" s="5" t="str">
         <f>B7</f>
         <v>그림 리퍼</v>
@@ -7220,7 +7217,7 @@
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B17" s="5" t="str">
         <f>B8</f>
         <v>파괴자 모로스</v>
@@ -7229,7 +7226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B18" s="25" t="str">
         <f>B9</f>
         <v>파괴자 모로스</v>
@@ -7238,7 +7235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B37" t="s">
         <v>86</v>
       </c>
@@ -7258,7 +7255,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>25</v>
       </c>
@@ -7280,7 +7277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B39" t="s">
         <v>91</v>
       </c>

</xml_diff>

<commit_message>
kmk - monster + dice bug fix
</commit_message>
<xml_diff>
--- a/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
+++ b/DarkDice/Assets/Scritable/Excel/DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Project\DarkDice\DarkDice\DarkDice\Assets\Scritable\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A614FAC9-487B-40D3-A842-08605AF42E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CEDCAA-9831-459F-A6DB-DC5A75D8F348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="855" activeTab="2" xr2:uid="{DC7D0983-50F2-4F61-969D-F2D36E7CA138}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="330">
   <si>
     <t>stage1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1159,9 +1159,6 @@
   </si>
   <si>
     <t>쉐도우</t>
-  </si>
-  <si>
-    <t>투헤드오크</t>
   </si>
   <si>
     <t>그림 리퍼</t>
@@ -2101,13 +2098,13 @@
     <xf numFmtId="49" fontId="13" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6223,30 +6220,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="25.2">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="2:9" ht="18" thickBot="1"/>
     <row r="4" spans="2:9" ht="19.8" thickBot="1">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="64"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="18"/>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="65"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="64"/>
+      <c r="I4" s="65"/>
     </row>
     <row r="5" spans="2:9" ht="19.8" thickBot="1">
       <c r="B5" s="12" t="s">
@@ -6355,10 +6352,10 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="19.8" thickBot="1">
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="64"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="18"/>
       <c r="E10" s="14" t="s">
         <v>15</v>
@@ -6412,10 +6409,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="64" t="s">
+      <c r="E13" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="64"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:9" ht="19.8" thickBot="1">
@@ -6447,10 +6444,10 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:9" ht="19.8" thickBot="1">
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -6464,10 +6461,10 @@
         <v>34</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="64" t="s">
+      <c r="E17" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="64"/>
+      <c r="F17" s="65"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -6505,10 +6502,10 @@
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="19.8" thickBot="1">
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="64"/>
+      <c r="C20" s="65"/>
       <c r="D20" s="18"/>
       <c r="E20" s="14" t="s">
         <v>38</v>
@@ -6632,6 +6629,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
@@ -6639,8 +6638,6 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6653,7 +6650,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
@@ -6737,10 +6734,10 @@
       </c>
       <c r="J2" s="58"/>
       <c r="K2" s="55" t="s">
+        <v>296</v>
+      </c>
+      <c r="L2" s="55" t="s">
         <v>297</v>
-      </c>
-      <c r="L2" s="55" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="19.2">
@@ -6758,7 +6755,7 @@
         <v>288</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F3" s="57"/>
       <c r="G3" s="57">
@@ -6774,7 +6771,7 @@
         <v>196</v>
       </c>
       <c r="K3" s="55" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L3" s="59"/>
     </row>
@@ -6790,13 +6787,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="55" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F4" s="57" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G4" s="57">
         <v>0</v>
@@ -6811,7 +6808,7 @@
         <v>143</v>
       </c>
       <c r="K4" s="55" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L4" s="55"/>
     </row>
@@ -6827,7 +6824,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E5" s="55"/>
       <c r="F5" s="57"/>
@@ -6844,7 +6841,7 @@
         <v>144</v>
       </c>
       <c r="K5" s="55" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L5" s="55"/>
     </row>
@@ -6860,13 +6857,13 @@
         <v>3</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F6" s="57" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G6" s="57">
         <v>0</v>
@@ -6879,7 +6876,7 @@
       </c>
       <c r="J6" s="58"/>
       <c r="K6" s="55" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L6" s="55"/>
     </row>
@@ -6914,7 +6911,7 @@
       </c>
       <c r="J7" s="58"/>
       <c r="K7" s="55" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L7" s="55"/>
     </row>
@@ -7004,10 +7001,10 @@
         <v>160</v>
       </c>
       <c r="J10" s="58" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K10" s="55" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L10" s="55"/>
     </row>
@@ -7041,7 +7038,7 @@
         <v>284</v>
       </c>
       <c r="L11" s="55" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="19.2">
@@ -7071,10 +7068,10 @@
       </c>
       <c r="J12" s="63"/>
       <c r="K12" s="56" t="s">
+        <v>305</v>
+      </c>
+      <c r="L12" s="56" t="s">
         <v>306</v>
-      </c>
-      <c r="L12" s="56" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="19.2">
@@ -7106,10 +7103,10 @@
       </c>
       <c r="J13" s="63"/>
       <c r="K13" s="56" t="s">
+        <v>307</v>
+      </c>
+      <c r="L13" s="56" t="s">
         <v>308</v>
-      </c>
-      <c r="L13" s="56" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="19.2">
@@ -7139,10 +7136,10 @@
       </c>
       <c r="J14" s="63"/>
       <c r="K14" s="56" t="s">
+        <v>309</v>
+      </c>
+      <c r="L14" s="56" t="s">
         <v>310</v>
-      </c>
-      <c r="L14" s="56" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="19.2">
@@ -7173,7 +7170,7 @@
         <v>200</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K15" s="56"/>
       <c r="L15" s="56"/>
@@ -7209,10 +7206,10 @@
       </c>
       <c r="J16" s="63"/>
       <c r="K16" s="56" t="s">
+        <v>311</v>
+      </c>
+      <c r="L16" s="56" t="s">
         <v>312</v>
-      </c>
-      <c r="L16" s="56" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="19.2">
@@ -7247,7 +7244,7 @@
       <c r="J17" s="63"/>
       <c r="K17" s="56"/>
       <c r="L17" s="56" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="19.2">
@@ -7293,7 +7290,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="56" t="s">
-        <v>294</v>
+        <v>239</v>
       </c>
       <c r="E19" s="56"/>
       <c r="F19" s="61"/>
@@ -7308,10 +7305,10 @@
       </c>
       <c r="J19" s="63"/>
       <c r="K19" s="56" t="s">
+        <v>314</v>
+      </c>
+      <c r="L19" s="56" t="s">
         <v>315</v>
-      </c>
-      <c r="L19" s="56" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="19.2">
@@ -7332,7 +7329,7 @@
         <v>293</v>
       </c>
       <c r="F20" s="61" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G20" s="61">
         <v>0</v>
@@ -7344,13 +7341,13 @@
         <v>240</v>
       </c>
       <c r="J20" s="63" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K20" s="56" t="s">
+        <v>316</v>
+      </c>
+      <c r="L20" s="56" t="s">
         <v>317</v>
-      </c>
-      <c r="L20" s="56" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="19.2">
@@ -7365,7 +7362,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E21" s="56"/>
       <c r="F21" s="61"/>
@@ -7380,10 +7377,10 @@
       </c>
       <c r="J21" s="63"/>
       <c r="K21" s="56" t="s">
+        <v>318</v>
+      </c>
+      <c r="L21" s="56" t="s">
         <v>319</v>
-      </c>
-      <c r="L21" s="56" t="s">
-        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -8109,7 +8106,7 @@
         <v>50</v>
       </c>
       <c r="H22" s="49" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I22" s="18"/>
       <c r="J22" s="18" t="s">
@@ -8207,7 +8204,7 @@
         <v>3417</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>194</v>
@@ -8720,7 +8717,7 @@
     </row>
     <row r="9" spans="2:17">
       <c r="B9" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C9" s="26">
         <v>23</v>

</xml_diff>